<commit_message>
test case - quiz
</commit_message>
<xml_diff>
--- a/TestCase.xlsx
+++ b/TestCase.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f2d0488956bc14b9/Documents/2021-Winter/4820/Behavior-Rating-tool/document/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="361" documentId="11_F25DC773A252ABDACC104826195E46E45BDE58EB" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{8DAB2895-3496-4923-8F64-7B03C4A6C7F1}"/>
+  <xr:revisionPtr revIDLastSave="415" documentId="11_F25DC773A252ABDACC104826195E46E45BDE58EB" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{2B232609-1BF8-47F6-BC1A-3B8EBC939022}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="user-creation" sheetId="6" r:id="rId1"/>
     <sheet name="login" sheetId="7" r:id="rId2"/>
     <sheet name="role-permission" sheetId="8" r:id="rId3"/>
-    <sheet name="template" sheetId="5" r:id="rId4"/>
+    <sheet name="quiz" sheetId="5" r:id="rId4"/>
+    <sheet name="template" sheetId="9" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="176">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -504,6 +505,111 @@
   </si>
   <si>
     <t>1. The users should receive email for reseting password</t>
+  </si>
+  <si>
+    <t>Admin create quiz</t>
+  </si>
+  <si>
+    <t>TA create quiz</t>
+  </si>
+  <si>
+    <t>Expert create quiz</t>
+  </si>
+  <si>
+    <t>add a new quiz</t>
+  </si>
+  <si>
+    <t>add new animal quiz</t>
+  </si>
+  <si>
+    <t>add/remove behviours</t>
+  </si>
+  <si>
+    <t>add/remove interpretations</t>
+  </si>
+  <si>
+    <t>upload videos</t>
+  </si>
+  <si>
+    <t>Edit quiz</t>
+  </si>
+  <si>
+    <t>different roles edit quiz</t>
+  </si>
+  <si>
+    <t>quiz-creation-001</t>
+  </si>
+  <si>
+    <t>admin review single</t>
+  </si>
+  <si>
+    <t>admin review all users</t>
+  </si>
+  <si>
+    <t>admin review a single user</t>
+  </si>
+  <si>
+    <t>download data</t>
+  </si>
+  <si>
+    <t>paging</t>
+  </si>
+  <si>
+    <t>search</t>
+  </si>
+  <si>
+    <t>test multiple pages</t>
+  </si>
+  <si>
+    <t>quiz-creation-002</t>
+  </si>
+  <si>
+    <t>quiz-creation-003</t>
+  </si>
+  <si>
+    <t>quiz-creation-004</t>
+  </si>
+  <si>
+    <t>quiz-creation-005</t>
+  </si>
+  <si>
+    <t>quiz-creation-006</t>
+  </si>
+  <si>
+    <t>quiz-creation-007</t>
+  </si>
+  <si>
+    <t>quiz-edition-008</t>
+  </si>
+  <si>
+    <t>quiz-edition-009</t>
+  </si>
+  <si>
+    <t>quiz-review-010</t>
+  </si>
+  <si>
+    <t>quiz-review-011</t>
+  </si>
+  <si>
+    <t>quiz-review-012</t>
+  </si>
+  <si>
+    <t>quiz-review-013</t>
+  </si>
+  <si>
+    <t>quiz-review-014</t>
+  </si>
+  <si>
+    <t>quiz-review-015</t>
+  </si>
+  <si>
+    <t>follow above 5 cases but using role of TA</t>
+  </si>
+  <si>
+    <t>follow above 5 cases but using role of Expert</t>
+  </si>
+  <si>
+    <t>search on a quiz, or user</t>
   </si>
 </sst>
 </file>
@@ -762,6 +868,22 @@
     <tableColumn id="5" xr3:uid="{85A29F9C-51A2-4554-B56C-98110F80668F}" name="Expected Result"/>
     <tableColumn id="6" xr3:uid="{21FA31DE-D880-4D07-8C47-C6497ED1A5C4}" name="Actual Result (Pass / Fail)"/>
     <tableColumn id="7" xr3:uid="{12B5E024-080C-4894-8479-95C86DFA5E9A}" name="option"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DE3DC403-CBCB-4CE6-8DCD-4207C00E5DE1}" name="Table42" displayName="Table42" ref="A1:G1048576" totalsRowShown="0">
+  <autoFilter ref="A1:G1048576" xr:uid="{4B5AE92E-4B21-45AF-829E-ACC7C40388B7}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{C1255A94-E784-4EDB-A629-8B10CCADA687}" name="Test Case ID"/>
+    <tableColumn id="2" xr3:uid="{E4EE8C65-27F1-4A0E-8BC6-7D7BFD50A3C7}" name="Scenario"/>
+    <tableColumn id="3" xr3:uid="{4AE36F0B-5338-47F7-860F-6CA321013146}" name="Test Case"/>
+    <tableColumn id="4" xr3:uid="{F2C8EA98-3A3F-4A09-846A-809E86045292}" name="Test Steps"/>
+    <tableColumn id="5" xr3:uid="{E98DECDE-8B01-4A5C-BF1E-C9F13A73B2A0}" name="Expected Result"/>
+    <tableColumn id="6" xr3:uid="{0F92F009-2A2F-429C-87A7-A09615BD6DF4}" name="Actual Result (Pass / Fail)"/>
+    <tableColumn id="7" xr3:uid="{3948F38B-7E9A-4502-87F7-A3306C3D9932}" name="option"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1032,9 +1154,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{862617E3-F5D8-4456-839B-FE1C3833AB05}">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K15" sqref="K15"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2360,14 +2482,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B251A65-4ED2-4229-84BD-0B0C4F5B3198}">
   <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
+      <selection pane="bottomLeft" activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="18.33203125" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" customWidth="1"/>
+    <col min="3" max="3" width="25.5546875" customWidth="1"/>
     <col min="4" max="4" width="25.21875" customWidth="1"/>
     <col min="5" max="5" width="28.5546875" customWidth="1"/>
     <col min="6" max="6" width="25.109375" customWidth="1"/>
@@ -2398,6 +2522,612 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A49" s="1"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A50" s="1"/>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A52" s="1"/>
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A53" s="1"/>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A54" s="1"/>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A0E8C0F-01A6-41A7-A0C4-7732268B6FE0}">
+  <dimension ref="A1:G54"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" customWidth="1"/>
+    <col min="3" max="3" width="25.5546875" customWidth="1"/>
+    <col min="4" max="4" width="25.21875" customWidth="1"/>
+    <col min="5" max="5" width="28.5546875" customWidth="1"/>
+    <col min="6" max="6" width="25.109375" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>

</xml_diff>

<commit_message>
test cases for Quiz - create/edit/review/take quiz
</commit_message>
<xml_diff>
--- a/TestCase.xlsx
+++ b/TestCase.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f2d0488956bc14b9/Documents/2021-Winter/4820/Behavior-Rating-tool/document/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="415" documentId="11_F25DC773A252ABDACC104826195E46E45BDE58EB" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{2B232609-1BF8-47F6-BC1A-3B8EBC939022}"/>
+  <xr:revisionPtr revIDLastSave="573" documentId="11_F25DC773A252ABDACC104826195E46E45BDE58EB" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{FAC3C36D-4A64-42E7-96E2-912FDA86096C}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="user-creation" sheetId="6" r:id="rId1"/>
     <sheet name="login" sheetId="7" r:id="rId2"/>
-    <sheet name="role-permission" sheetId="8" r:id="rId3"/>
-    <sheet name="quiz" sheetId="5" r:id="rId4"/>
+    <sheet name="quiz" sheetId="5" r:id="rId3"/>
+    <sheet name="role-permission" sheetId="8" r:id="rId4"/>
     <sheet name="template" sheetId="9" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="236">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -531,78 +531,9 @@
     <t>upload videos</t>
   </si>
   <si>
-    <t>Edit quiz</t>
-  </si>
-  <si>
-    <t>different roles edit quiz</t>
-  </si>
-  <si>
-    <t>quiz-creation-001</t>
-  </si>
-  <si>
-    <t>admin review single</t>
-  </si>
-  <si>
-    <t>admin review all users</t>
-  </si>
-  <si>
-    <t>admin review a single user</t>
-  </si>
-  <si>
-    <t>download data</t>
-  </si>
-  <si>
-    <t>paging</t>
-  </si>
-  <si>
-    <t>search</t>
-  </si>
-  <si>
     <t>test multiple pages</t>
   </si>
   <si>
-    <t>quiz-creation-002</t>
-  </si>
-  <si>
-    <t>quiz-creation-003</t>
-  </si>
-  <si>
-    <t>quiz-creation-004</t>
-  </si>
-  <si>
-    <t>quiz-creation-005</t>
-  </si>
-  <si>
-    <t>quiz-creation-006</t>
-  </si>
-  <si>
-    <t>quiz-creation-007</t>
-  </si>
-  <si>
-    <t>quiz-edition-008</t>
-  </si>
-  <si>
-    <t>quiz-edition-009</t>
-  </si>
-  <si>
-    <t>quiz-review-010</t>
-  </si>
-  <si>
-    <t>quiz-review-011</t>
-  </si>
-  <si>
-    <t>quiz-review-012</t>
-  </si>
-  <si>
-    <t>quiz-review-013</t>
-  </si>
-  <si>
-    <t>quiz-review-014</t>
-  </si>
-  <si>
-    <t>quiz-review-015</t>
-  </si>
-  <si>
     <t>follow above 5 cases but using role of TA</t>
   </si>
   <si>
@@ -610,6 +541,295 @@
   </si>
   <si>
     <t>search on a quiz, or user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>A new quiz is created, users can conduct the quiz and answer saved</t>
+  </si>
+  <si>
+    <t>1. In the Create new Quiz page, in the bottom left, add a new animal by the 'Edit me..' single selection input box
+2. Or select an existing animal.</t>
+  </si>
+  <si>
+    <t>The new animal should be added to the system</t>
+  </si>
+  <si>
+    <t>1. In the Create new Quiz page, focus on the Behaviours section, using the Edit me… checkbox input box to add Behaviours, and check on the solution answers.
+2. if the given checkbox options are not enough, use the add or remove button to add more (or reduce to less)</t>
+  </si>
+  <si>
+    <t>All the behavior options should be added and the checked solution should be saved</t>
+  </si>
+  <si>
+    <t>All the Interpretation options should be added and the selected solution should be saved</t>
+  </si>
+  <si>
+    <t>1. In the Create new Quiz page, focus on the Interpretation section, using the Edit me… input box to add Interpretation, and select the solution answer.
+2. if the given checkbox options are not enough, use the add or remove button to add more (or reduce to less)</t>
+  </si>
+  <si>
+    <t>1. In the Create New Quiz page top-left Import video panel, click on the Browse button to select a video clip of animal behaviors then click on the upload button to upload.
+2. In the Video information section, specify a video name for it or leave it automatically.</t>
+  </si>
+  <si>
+    <t>The video clip would be uploaded and the video information would be be saved</t>
+  </si>
+  <si>
+    <t>1. login as admin
+2. go to the Quizzes page and click on the Create New Quiz
+3. Then follow the instructions to create a new quiz including animal, video, behaviors and interpretation, details will be described in the cases below. Then click on the Create Quiz button to save the quiz.</t>
+  </si>
+  <si>
+    <t>Login as an Expert user, then follow the abovec 5 steps to create a new quiz.</t>
+  </si>
+  <si>
+    <t>Login as a TA user, then follow the abovec 5 steps to create a new quiz.</t>
+  </si>
+  <si>
+    <t>Admin Edit quiz</t>
+  </si>
+  <si>
+    <t>TA Edit quiz</t>
+  </si>
+  <si>
+    <t>Expert Edit quiz</t>
+  </si>
+  <si>
+    <t>Quiz-Creation-001</t>
+  </si>
+  <si>
+    <t>Quiz-Creation-002</t>
+  </si>
+  <si>
+    <t>Quiz-Creation-003</t>
+  </si>
+  <si>
+    <t>Quiz-Creation-004</t>
+  </si>
+  <si>
+    <t>Quiz-Creation-005</t>
+  </si>
+  <si>
+    <t>Quiz-Creation-006</t>
+  </si>
+  <si>
+    <t>Quiz-Creation-007</t>
+  </si>
+  <si>
+    <t>Admin edit existing quiz</t>
+  </si>
+  <si>
+    <t>All the changes that should be applied to the quiz after Clicking on the Edit Quiz.</t>
+  </si>
+  <si>
+    <t>The current system didn't consider the already conducted quiz when Editing the Quiz. This means after Editing the quiz, such as changed the solution answer, then the Scores will NOT be recalculated, they are not refershed when Editing Quiz. But this can be achieved by a script, or add a button as Apply Editing Quiz to exising quizzes.</t>
+  </si>
+  <si>
+    <t>1. Login as an admin user
+2. Select the Quizzes page, and choose an existing target quiz, then click on the Edit Quiz button
+3. In the Edit Quiz page, do the following changes:
+a. Change the Video Name; 
+b. Change the Animal information; 
+c. add more or reduce less Behavior options; 
+d. Change berhavior solution answers; 
+e. Change the interpretations (add and reduce);
+f. Change the interpretation solution answers</t>
+  </si>
+  <si>
+    <t>TA edit existing quiz</t>
+  </si>
+  <si>
+    <t>Expert edit existing quiz</t>
+  </si>
+  <si>
+    <t>1. Login as a TA user
+2. Follow the same step as above admin Edit quiz</t>
+  </si>
+  <si>
+    <t>1. Login as an Expert user
+2. Follow the same step as above admin Edit quiz</t>
+  </si>
+  <si>
+    <t>Quiz-Edition-008</t>
+  </si>
+  <si>
+    <t>Quiz-Edition-009</t>
+  </si>
+  <si>
+    <t>Quiz-Edition-010</t>
+  </si>
+  <si>
+    <t>The user should not see the Edit quiz or Create quiz button on the Quizzes page</t>
+  </si>
+  <si>
+    <t>Other roles edit quiz</t>
+  </si>
+  <si>
+    <t>Other roles (student..) can't see Edit Quiz button</t>
+  </si>
+  <si>
+    <t>1. Login as a student account
+2. The user should not see the Edit quiz nor Create quiz button on the Quizzes page</t>
+  </si>
+  <si>
+    <t>Users review my quizzes</t>
+  </si>
+  <si>
+    <t>Admin review all users quizzes</t>
+  </si>
+  <si>
+    <t>Admin review a single user quizzes</t>
+  </si>
+  <si>
+    <t>Download data</t>
+  </si>
+  <si>
+    <t>Paging</t>
+  </si>
+  <si>
+    <t>Search</t>
+  </si>
+  <si>
+    <t>Download data, CSV and JSON</t>
+  </si>
+  <si>
+    <t>User-019</t>
+  </si>
+  <si>
+    <t>download users</t>
+  </si>
+  <si>
+    <t>download users as csv and Json</t>
+  </si>
+  <si>
+    <t>1. login as an admin, or TA
+2. in the Users page, there is a Download button
+3. Download users a CSV or Json, all the users should be included in the file with their role, grad_year and personal information.</t>
+  </si>
+  <si>
+    <t>The files should be downloaded, all the users should be included with the information</t>
+  </si>
+  <si>
+    <t>Review a quiz page</t>
+  </si>
+  <si>
+    <t>Review a single quiz</t>
+  </si>
+  <si>
+    <t>1. select any quiz to review
+2. the corrected answer should be marked as green, and it will also tells that if you did wrong on the behaviors or interpretations.
+3. And those answers are no changeable.</t>
+  </si>
+  <si>
+    <t>Users got what they selected during the quiz, and got informed which got right and wrong.</t>
+  </si>
+  <si>
+    <t>Users would see a list of quiz attempts that they conducted in the review table, and clicking on the link can check the quiz details.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Login as any roles
+2. Open the Review page
+3. In the Review My Quiz section, users can see their conducted quiz list with all the attempts.
+4. click on the link of each attempt, they can check the details of how they answered during the quiz. </t>
+  </si>
+  <si>
+    <t>1. Login as Admin or TA
+2. Go the Review page
+3. In the second table, the Review All Student Quizzes section, there is a list of all the quiz attempts that conducted by all the users.
+4. By clicking on a user name link, a full table of quiz attempts by that user will be listed.
+5. By clicking on a quiz code link, a full table of that specific quiz that conducted by any users will be listed.</t>
+  </si>
+  <si>
+    <t>1. Login as Admin or TA
+2. Go the Review page
+3. In the second table, the Review All Student Quizzes section, there is a list of all the quiz attempts that conducted by all the users.
+4. By clicking on a user name link, a full table of quiz attempts by that user will be listed.</t>
+  </si>
+  <si>
+    <t>Admin or TA can check all the student quiz attempts, based on users or quiz code.</t>
+  </si>
+  <si>
+    <t>Download review data is avilable on the Review All Student Quizzes table, both CSV and JSON supported</t>
+  </si>
+  <si>
+    <t>CSV and JSON formate can be downloaded for all the user quiz attemps</t>
+  </si>
+  <si>
+    <t>This download always shows all the users all the quizzes, this will not be match with the Search result.</t>
+  </si>
+  <si>
+    <t>1. Prepare more data, conducting different quizzes, as different users.
+2. Then using the search function based on username, quiz code, and so on to check the result</t>
+  </si>
+  <si>
+    <t>Search result should be working as expected</t>
+  </si>
+  <si>
+    <t>Paging should be working as expected</t>
+  </si>
+  <si>
+    <t>1. Prepare more data, conducting different quizzes, as different users.
+2. Then try the paging function, go to next page, previous page to check the data
+3. Specify Show .. Entities, and check the rows per page is showed as the number specified.</t>
+  </si>
+  <si>
+    <t>Conducting quiz</t>
+  </si>
+  <si>
+    <t>Conducting quiz - empty</t>
+  </si>
+  <si>
+    <t>Conducting quiz - answers</t>
+  </si>
+  <si>
+    <t>1. Login as any roles (try different roles)
+2. Then select the Quizzes page
+3. choose a target quiz, then click on the Take Quiz button
+4. Watch the video, not select any answers, and submit</t>
+  </si>
+  <si>
+    <t>can not be submit without any answer selected, and got warning of what should do.</t>
+  </si>
+  <si>
+    <t>1. Login as any roles (try different roles)
+2. Then select the Quizzes page
+3. choose a target quiz, then click on the Take Quiz button
+4. Watch the video, select Behaviours, and interpretation and click on Submit Responses.</t>
+  </si>
+  <si>
+    <t>Quiz should be submited and saved in the database, Users can review it in the reiew page correctly.</t>
+  </si>
+  <si>
+    <t>Quiz-Edition-011</t>
+  </si>
+  <si>
+    <t>Quiz-Review-010</t>
+  </si>
+  <si>
+    <t>Quiz-Review-011</t>
+  </si>
+  <si>
+    <t>Quiz-Review-012</t>
+  </si>
+  <si>
+    <t>Quiz-Review-013</t>
+  </si>
+  <si>
+    <t>Quiz-Review-014</t>
+  </si>
+  <si>
+    <t>Quiz-Review-015</t>
+  </si>
+  <si>
+    <t>Quiz-Review-016</t>
+  </si>
+  <si>
+    <t>Quiz-Taken-017</t>
+  </si>
+  <si>
+    <t>Quiz-Taken-018</t>
   </si>
 </sst>
 </file>
@@ -744,7 +964,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -768,6 +988,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -780,11 +1006,41 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="18">
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -842,32 +1098,32 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{65197289-B2F1-4FBA-A410-1F433A75918A}" name="Table47" displayName="Table47" ref="A1:G1048556" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{65197289-B2F1-4FBA-A410-1F433A75918A}" name="Table47" displayName="Table47" ref="A1:G1048556" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <autoFilter ref="A1:G1048556" xr:uid="{5C0A8A10-CE36-4D89-A192-0010E1BF81CD}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{3A8F5125-A564-4E66-8567-8CDC78EA1CB4}" name="Test Case ID" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{E19BD2D7-3CFE-404D-995F-3DAF2B1C95B2}" name="Scenario" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{41869099-DCAF-4719-8901-EBD55DA565DC}" name="Test Case" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{B02E3273-7B16-4429-BFE1-4EA15BB30C99}" name="Test Steps" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{E2E76E0A-8EF6-40DA-8BEB-5EF2FD0DBC3F}" name="Expected Result" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{2CC81B51-C339-4EC6-B2FA-C34EF60AEDFB}" name="Actual Result (Pass / Fail)" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{1249CAEA-7296-4AE6-AE7D-6C5C9C29D3DA}" name="option" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{3A8F5125-A564-4E66-8567-8CDC78EA1CB4}" name="Test Case ID" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{E19BD2D7-3CFE-404D-995F-3DAF2B1C95B2}" name="Scenario" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{41869099-DCAF-4719-8901-EBD55DA565DC}" name="Test Case" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{B02E3273-7B16-4429-BFE1-4EA15BB30C99}" name="Test Steps" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{E2E76E0A-8EF6-40DA-8BEB-5EF2FD0DBC3F}" name="Expected Result" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{2CC81B51-C339-4EC6-B2FA-C34EF60AEDFB}" name="Actual Result (Pass / Fail)" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{1249CAEA-7296-4AE6-AE7D-6C5C9C29D3DA}" name="option" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{92AC25D0-1840-40EF-957E-647187AF8E3F}" name="Table4" displayName="Table4" ref="A1:G1048576" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{92AC25D0-1840-40EF-957E-647187AF8E3F}" name="Table4" displayName="Table4" ref="A1:G1048576" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="A1:G1048576" xr:uid="{8B347093-EBF6-4926-BF9C-4D3D7772951F}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{8776D5CD-5A3D-46B8-B7F7-46084F76F8E6}" name="Test Case ID"/>
-    <tableColumn id="2" xr3:uid="{4A7F3797-150E-41A8-9565-29A5721E62D9}" name="Scenario"/>
-    <tableColumn id="3" xr3:uid="{40DD4476-21C0-495D-BE46-E47BFCBA7F01}" name="Test Case"/>
-    <tableColumn id="4" xr3:uid="{9569C168-520F-404E-B2B2-9CAD0036A4B0}" name="Test Steps"/>
-    <tableColumn id="5" xr3:uid="{85A29F9C-51A2-4554-B56C-98110F80668F}" name="Expected Result"/>
-    <tableColumn id="6" xr3:uid="{21FA31DE-D880-4D07-8C47-C6497ED1A5C4}" name="Actual Result (Pass / Fail)"/>
-    <tableColumn id="7" xr3:uid="{12B5E024-080C-4894-8479-95C86DFA5E9A}" name="option"/>
+    <tableColumn id="1" xr3:uid="{8776D5CD-5A3D-46B8-B7F7-46084F76F8E6}" name="Test Case ID" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{4A7F3797-150E-41A8-9565-29A5721E62D9}" name="Scenario" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{40DD4476-21C0-495D-BE46-E47BFCBA7F01}" name="Test Case" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{9569C168-520F-404E-B2B2-9CAD0036A4B0}" name="Test Steps" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{85A29F9C-51A2-4554-B56C-98110F80668F}" name="Expected Result" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{21FA31DE-D880-4D07-8C47-C6497ED1A5C4}" name="Actual Result (Pass / Fail)" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{12B5E024-080C-4894-8479-95C86DFA5E9A}" name="option" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1155,8 +1411,8 @@
   <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J6" sqref="J6"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1541,14 +1797,24 @@
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
+    <row r="20" spans="1:7" s="11" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
@@ -1677,6 +1943,7 @@
       <c r="G34" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -2125,11 +2392,743 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B251A65-4ED2-4229-84BD-0B0C4F5B3198}">
+  <dimension ref="A1:G54"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.33203125" style="11" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" style="11" customWidth="1"/>
+    <col min="3" max="3" width="25.5546875" style="11" customWidth="1"/>
+    <col min="4" max="4" width="42.109375" style="11" customWidth="1"/>
+    <col min="5" max="5" width="28.5546875" style="11" customWidth="1"/>
+    <col min="6" max="6" width="25.109375" style="11" customWidth="1"/>
+    <col min="7" max="7" width="49.21875" style="11" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="17" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" s="17" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" s="17" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" s="17" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" s="17" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" s="17" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" s="17" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" s="17" customFormat="1" ht="144" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="17" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" s="17" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" s="17" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" s="17" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" s="17" customFormat="1" ht="144" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" s="17" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" s="17" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="1:7" s="17" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" s="17" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="1:7" s="17" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="1:7" s="17" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="1:7" s="17" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+    </row>
+    <row r="24" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+    </row>
+    <row r="25" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+    </row>
+    <row r="26" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+    </row>
+    <row r="27" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+    </row>
+    <row r="28" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+    </row>
+    <row r="29" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+    </row>
+    <row r="30" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+    </row>
+    <row r="31" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+    </row>
+    <row r="32" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+    </row>
+    <row r="33" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+    </row>
+    <row r="34" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+    </row>
+    <row r="35" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" s="12"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" s="12"/>
+      <c r="B37" s="12"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="12"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" s="12"/>
+      <c r="B38" s="12"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="12"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" s="12"/>
+      <c r="B39" s="12"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="12"/>
+      <c r="G39" s="12"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" s="12"/>
+      <c r="B40" s="12"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="12"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" s="12"/>
+      <c r="B41" s="12"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="12"/>
+      <c r="F41" s="12"/>
+      <c r="G41" s="12"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" s="12"/>
+      <c r="B42" s="12"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="12"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43" s="12"/>
+      <c r="B43" s="12"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="12"/>
+      <c r="F43" s="12"/>
+      <c r="G43" s="12"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44" s="12"/>
+      <c r="B44" s="12"/>
+      <c r="C44" s="12"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="12"/>
+      <c r="G44" s="12"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45" s="12"/>
+      <c r="B45" s="12"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="12"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46" s="12"/>
+      <c r="B46" s="12"/>
+      <c r="C46" s="12"/>
+      <c r="D46" s="12"/>
+      <c r="E46" s="12"/>
+      <c r="F46" s="12"/>
+      <c r="G46" s="12"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" s="12"/>
+      <c r="B47" s="12"/>
+      <c r="C47" s="12"/>
+      <c r="D47" s="12"/>
+      <c r="E47" s="12"/>
+      <c r="F47" s="12"/>
+      <c r="G47" s="12"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48" s="12"/>
+      <c r="B48" s="12"/>
+      <c r="C48" s="12"/>
+      <c r="D48" s="12"/>
+      <c r="E48" s="12"/>
+      <c r="F48" s="12"/>
+      <c r="G48" s="12"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A49" s="12"/>
+      <c r="B49" s="12"/>
+      <c r="C49" s="12"/>
+      <c r="D49" s="12"/>
+      <c r="E49" s="12"/>
+      <c r="F49" s="12"/>
+      <c r="G49" s="12"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A50" s="12"/>
+      <c r="B50" s="12"/>
+      <c r="C50" s="12"/>
+      <c r="D50" s="12"/>
+      <c r="E50" s="12"/>
+      <c r="F50" s="12"/>
+      <c r="G50" s="12"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A51" s="12"/>
+      <c r="B51" s="12"/>
+      <c r="C51" s="12"/>
+      <c r="D51" s="12"/>
+      <c r="E51" s="12"/>
+      <c r="F51" s="12"/>
+      <c r="G51" s="12"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A52" s="12"/>
+      <c r="B52" s="12"/>
+      <c r="C52" s="12"/>
+      <c r="D52" s="12"/>
+      <c r="E52" s="12"/>
+      <c r="F52" s="12"/>
+      <c r="G52" s="12"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A53" s="12"/>
+      <c r="B53" s="12"/>
+      <c r="C53" s="12"/>
+      <c r="D53" s="12"/>
+      <c r="E53" s="12"/>
+      <c r="F53" s="12"/>
+      <c r="G53" s="12"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A54" s="12"/>
+      <c r="B54" s="12"/>
+      <c r="C54" s="12"/>
+      <c r="D54" s="12"/>
+      <c r="E54" s="12"/>
+      <c r="F54" s="12"/>
+      <c r="G54" s="12"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{758DE97B-9417-4FE9-AABB-4BFFC9BE7D63}">
   <dimension ref="A1:C46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2140,11 +3139,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
     </row>
     <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
@@ -2158,7 +3157,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="14" t="s">
         <v>103</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -2167,21 +3166,21 @@
       <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="13"/>
+      <c r="A4" s="15"/>
       <c r="B4" s="3" t="s">
         <v>88</v>
       </c>
       <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="13"/>
+      <c r="A5" s="15"/>
       <c r="B5" s="3" t="s">
         <v>89</v>
       </c>
       <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="14"/>
+      <c r="A6" s="16"/>
       <c r="B6" s="3" t="s">
         <v>90</v>
       </c>
@@ -2193,7 +3192,7 @@
       <c r="C7" s="6"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="14" t="s">
         <v>104</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -2202,35 +3201,35 @@
       <c r="C8" s="3"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="13"/>
+      <c r="A9" s="15"/>
       <c r="B9" s="3" t="s">
         <v>88</v>
       </c>
       <c r="C9" s="3"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="13"/>
+      <c r="A10" s="15"/>
       <c r="B10" s="3" t="s">
         <v>91</v>
       </c>
       <c r="C10" s="3"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="13"/>
+      <c r="A11" s="15"/>
       <c r="B11" s="3" t="s">
         <v>92</v>
       </c>
       <c r="C11" s="3"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="13"/>
+      <c r="A12" s="15"/>
       <c r="B12" s="3" t="s">
         <v>89</v>
       </c>
       <c r="C12" s="3"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="14"/>
+      <c r="A13" s="16"/>
       <c r="B13" s="3" t="s">
         <v>90</v>
       </c>
@@ -2242,7 +3241,7 @@
       <c r="C14" s="6"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="14" t="s">
         <v>105</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -2251,63 +3250,63 @@
       <c r="C15" s="3"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="13"/>
+      <c r="A16" s="15"/>
       <c r="B16" s="3" t="s">
         <v>94</v>
       </c>
       <c r="C16" s="3"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="13"/>
+      <c r="A17" s="15"/>
       <c r="B17" s="3" t="s">
         <v>95</v>
       </c>
       <c r="C17" s="3"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="13"/>
+      <c r="A18" s="15"/>
       <c r="B18" s="3" t="s">
         <v>96</v>
       </c>
       <c r="C18" s="3"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="13"/>
+      <c r="A19" s="15"/>
       <c r="B19" s="3" t="s">
         <v>97</v>
       </c>
       <c r="C19" s="3"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="13"/>
+      <c r="A20" s="15"/>
       <c r="B20" s="3" t="s">
         <v>87</v>
       </c>
       <c r="C20" s="3"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="13"/>
+      <c r="A21" s="15"/>
       <c r="B21" s="3" t="s">
         <v>88</v>
       </c>
       <c r="C21" s="3"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="13"/>
+      <c r="A22" s="15"/>
       <c r="B22" s="3" t="s">
         <v>91</v>
       </c>
       <c r="C22" s="3"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="13"/>
+      <c r="A23" s="15"/>
       <c r="B23" s="3" t="s">
         <v>92</v>
       </c>
       <c r="C23" s="3"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="13"/>
+      <c r="A24" s="15"/>
       <c r="B24" s="3" t="s">
         <v>109</v>
       </c>
@@ -2316,7 +3315,7 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="13"/>
+      <c r="A25" s="15"/>
       <c r="B25" s="3" t="s">
         <v>110</v>
       </c>
@@ -2325,14 +3324,14 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="13"/>
+      <c r="A26" s="15"/>
       <c r="B26" s="3" t="s">
         <v>98</v>
       </c>
       <c r="C26" s="3"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="14"/>
+      <c r="A27" s="16"/>
       <c r="B27" s="3" t="s">
         <v>90</v>
       </c>
@@ -2344,7 +3343,7 @@
       <c r="C28" s="6"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="12" t="s">
+      <c r="A29" s="14" t="s">
         <v>106</v>
       </c>
       <c r="B29" s="3" t="s">
@@ -2353,98 +3352,98 @@
       <c r="C29" s="3"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="13"/>
+      <c r="A30" s="15"/>
       <c r="B30" s="3" t="s">
         <v>94</v>
       </c>
       <c r="C30" s="3"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="13"/>
+      <c r="A31" s="15"/>
       <c r="B31" s="3" t="s">
         <v>95</v>
       </c>
       <c r="C31" s="3"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="13"/>
+      <c r="A32" s="15"/>
       <c r="B32" s="3" t="s">
         <v>99</v>
       </c>
       <c r="C32" s="3"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="13"/>
+      <c r="A33" s="15"/>
       <c r="B33" s="3" t="s">
         <v>96</v>
       </c>
       <c r="C33" s="3"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="13"/>
+      <c r="A34" s="15"/>
       <c r="B34" s="3" t="s">
         <v>97</v>
       </c>
       <c r="C34" s="3"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="13"/>
+      <c r="A35" s="15"/>
       <c r="B35" s="3" t="s">
         <v>87</v>
       </c>
       <c r="C35" s="3"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="13"/>
+      <c r="A36" s="15"/>
       <c r="B36" s="3" t="s">
         <v>88</v>
       </c>
       <c r="C36" s="3"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="13"/>
+      <c r="A37" s="15"/>
       <c r="B37" s="3" t="s">
         <v>91</v>
       </c>
       <c r="C37" s="3"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="13"/>
+      <c r="A38" s="15"/>
       <c r="B38" s="3" t="s">
         <v>92</v>
       </c>
       <c r="C38" s="3"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" s="13"/>
+      <c r="A39" s="15"/>
       <c r="B39" s="3" t="s">
         <v>100</v>
       </c>
       <c r="C39" s="3"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" s="13"/>
+      <c r="A40" s="15"/>
       <c r="B40" s="3" t="s">
         <v>89</v>
       </c>
       <c r="C40" s="3"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" s="13"/>
+      <c r="A41" s="15"/>
       <c r="B41" s="3" t="s">
         <v>101</v>
       </c>
       <c r="C41" s="3"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" s="13"/>
+      <c r="A42" s="15"/>
       <c r="B42" s="3" t="s">
         <v>98</v>
       </c>
       <c r="C42" s="3"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" s="14"/>
+      <c r="A43" s="16"/>
       <c r="B43" s="3" t="s">
         <v>102</v>
       </c>
@@ -2475,613 +3474,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B251A65-4ED2-4229-84BD-0B0C4F5B3198}">
-  <dimension ref="A1:G54"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C34" sqref="C34"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="18.33203125" customWidth="1"/>
-    <col min="2" max="2" width="23.33203125" customWidth="1"/>
-    <col min="3" max="3" width="25.5546875" customWidth="1"/>
-    <col min="4" max="4" width="25.21875" customWidth="1"/>
-    <col min="5" max="5" width="28.5546875" customWidth="1"/>
-    <col min="6" max="6" width="25.109375" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" s="1"/>
-      <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" s="1"/>
-      <c r="B48" s="1"/>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
-      <c r="G48" s="1"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49" s="1"/>
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
-      <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A50" s="1"/>
-      <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
-      <c r="F50" s="1"/>
-      <c r="G50" s="1"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A51" s="1"/>
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
-      <c r="E51" s="1"/>
-      <c r="F51" s="1"/>
-      <c r="G51" s="1"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A52" s="1"/>
-      <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
-      <c r="F52" s="1"/>
-      <c r="G52" s="1"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A53" s="1"/>
-      <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A54" s="1"/>
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
-      <c r="F54" s="1"/>
-      <c r="G54" s="1"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>